<commit_message>
handle dividion by 0 and output step with no previous steps
</commit_message>
<xml_diff>
--- a/project-manager/project-manager/Tests.xlsx
+++ b/project-manager/project-manager/Tests.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/victorstefan/Documents/Proiecte/Facultate/Project-manager/project-manager/project-manager/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B615C576-1B7B-6C48-8D58-8D0C6AEF0E16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8E0AF02-3563-2D41-8ED4-31D308AF32A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="840" windowWidth="38400" windowHeight="24020" xr2:uid="{8D6A7EFB-34E7-E148-9BC7-7EF0A9AE5FB8}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="49">
   <si>
     <t>The app worked correctly for the folowing tests</t>
   </si>
@@ -115,12 +115,6 @@
     <t>Calculus(Step 2)(1)</t>
   </si>
   <si>
-    <t>1. Number(description1)(0)(0)</t>
-  </si>
-  <si>
-    <t>3. Number(description1)(11)(1)</t>
-  </si>
-  <si>
     <t>Calculus()(Step 1, Step 2)(1)</t>
   </si>
   <si>
@@ -163,7 +157,31 @@
     <t>2. Calculus()(2 random steps)</t>
   </si>
   <si>
-    <t>4. Output(all previous steps)</t>
+    <t>2. Calculus()(Step 1)(1)</t>
+  </si>
+  <si>
+    <t>3. Output(all previous steps)</t>
+  </si>
+  <si>
+    <t>3. Number(description2)(22)(1)</t>
+  </si>
+  <si>
+    <t>3. Number(description3)(11)(1)</t>
+  </si>
+  <si>
+    <t>2. CsvFile(description2)(test.csv)(0)</t>
+  </si>
+  <si>
+    <t>4. Entered bad input a couple of times</t>
+  </si>
+  <si>
+    <t>5. Ran flow analysis(details) option</t>
+  </si>
+  <si>
+    <t>1. Number(description1)(111)(1)</t>
+  </si>
+  <si>
+    <t>3. Number(description2)(0)(0)</t>
   </si>
 </sst>
 </file>
@@ -518,7 +536,7 @@
   <dimension ref="A1:F24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -526,8 +544,8 @@
     <col min="2" max="2" width="31" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="31.83203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="40.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="31.5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="21.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="33" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="30.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
@@ -537,7 +555,7 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
@@ -682,13 +700,13 @@
         <v>10</v>
       </c>
       <c r="B14" t="s">
+        <v>47</v>
+      </c>
+      <c r="C14" t="s">
+        <v>48</v>
+      </c>
+      <c r="D14" t="s">
         <v>26</v>
-      </c>
-      <c r="C14" t="s">
-        <v>27</v>
-      </c>
-      <c r="D14" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
@@ -702,13 +720,13 @@
         <v>9</v>
       </c>
       <c r="D15" t="s">
+        <v>27</v>
+      </c>
+      <c r="E15" t="s">
+        <v>28</v>
+      </c>
+      <c r="F15" t="s">
         <v>29</v>
-      </c>
-      <c r="E15" t="s">
-        <v>30</v>
-      </c>
-      <c r="F15" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
@@ -716,16 +734,16 @@
         <v>12</v>
       </c>
       <c r="B16" t="s">
+        <v>31</v>
+      </c>
+      <c r="C16" t="s">
+        <v>32</v>
+      </c>
+      <c r="D16" t="s">
         <v>33</v>
       </c>
-      <c r="C16" t="s">
-        <v>34</v>
-      </c>
-      <c r="D16" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>13</v>
       </c>
@@ -736,18 +754,18 @@
         <v>9</v>
       </c>
       <c r="D17" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>14</v>
       </c>
       <c r="B18" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>15</v>
       </c>
@@ -755,45 +773,72 @@
         <v>2</v>
       </c>
       <c r="C19" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D19" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E19" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>16</v>
       </c>
       <c r="B20" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C20" t="s">
+        <v>39</v>
+      </c>
+      <c r="D20" t="s">
         <v>41</v>
       </c>
-      <c r="D20" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>17</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B21" t="s">
+        <v>5</v>
+      </c>
+      <c r="C21" t="s">
+        <v>40</v>
+      </c>
+      <c r="D21" t="s">
+        <v>42</v>
+      </c>
+      <c r="E21" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>18</v>
       </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B22" t="s">
+        <v>8</v>
+      </c>
+      <c r="C22" t="s">
+        <v>44</v>
+      </c>
+      <c r="D22" t="s">
+        <v>43</v>
+      </c>
+      <c r="E22" t="s">
+        <v>45</v>
+      </c>
+      <c r="F22" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>19</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>20</v>
       </c>

</xml_diff>

<commit_message>
tests are done, added a few more error handlers
</commit_message>
<xml_diff>
--- a/project-manager/project-manager/Tests.xlsx
+++ b/project-manager/project-manager/Tests.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/victorstefan/Documents/Proiecte/Facultate/Project-manager/project-manager/project-manager/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8E0AF02-3563-2D41-8ED4-31D308AF32A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A463322-E7DD-A74A-A106-3539764AD1AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="840" windowWidth="38400" windowHeight="24020" xr2:uid="{8D6A7EFB-34E7-E148-9BC7-7EF0A9AE5FB8}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="76">
   <si>
     <t>The app worked correctly for the folowing tests</t>
   </si>
@@ -79,9 +79,6 @@
     <t>3. Calculus()()(1)</t>
   </si>
   <si>
-    <t>4. TextInput(description)(some random text)(1)</t>
-  </si>
-  <si>
     <t>4. Output()(Steps 1, 2 and 3)</t>
   </si>
   <si>
@@ -106,9 +103,6 @@
     <t>2. Entered some bad input for Step 1</t>
   </si>
   <si>
-    <t>1. Display()()(1)</t>
-  </si>
-  <si>
     <t>2. Number(description)(22)(1)</t>
   </si>
   <si>
@@ -182,6 +176,93 @@
   </si>
   <si>
     <t>3. Number(description2)(0)(0)</t>
+  </si>
+  <si>
+    <t>1. Output()()(1)</t>
+  </si>
+  <si>
+    <t>1. Added one of each flow, 2 Numbers</t>
+  </si>
+  <si>
+    <t>2. Entered some bad inputs where I could</t>
+  </si>
+  <si>
+    <t>4. Deleted the flow</t>
+  </si>
+  <si>
+    <t>5. Tried to run it again</t>
+  </si>
+  <si>
+    <t>A step with 0 as the number of times executed means it was skipped</t>
+  </si>
+  <si>
+    <t>The goals of each step</t>
+  </si>
+  <si>
+    <t>Check if Title, Text and TextInput creation / execution work correctly</t>
+  </si>
+  <si>
+    <t>Check Number and Calculus Steps, if calculus can get the previous number steps as parameters</t>
+  </si>
+  <si>
+    <t>See if TextFile and CsvFile work as expected and Display can receive them as parameters</t>
+  </si>
+  <si>
+    <t>Check Calculus with no previous Number Steps</t>
+  </si>
+  <si>
+    <t>Run Output for Title, Text and TextInput, to see if they are added to the file as expected</t>
+  </si>
+  <si>
+    <t>Ran Display with no previous TextFile or CsvFile, and checked if Output adds Number and Calculus to the file as it should</t>
+  </si>
+  <si>
+    <t>Checked if the flow analytis for Number work as they should</t>
+  </si>
+  <si>
+    <t>Ran Calculus with no previous Number steps</t>
+  </si>
+  <si>
+    <t>Checked if division by 0 si handled well</t>
+  </si>
+  <si>
+    <t>Added 2 of each file type to see if Display can display any of them</t>
+  </si>
+  <si>
+    <t>Wanted to see if a flow is deleted correctly</t>
+  </si>
+  <si>
+    <t>Checked if TextFile and CsvFile are added to the Output file as expected</t>
+  </si>
+  <si>
+    <t>Ran Calculus with only one previous Number step</t>
+  </si>
+  <si>
+    <t>Checked if Calculus works well with a lot of previous Numbers</t>
+  </si>
+  <si>
+    <t>Executed the second Number step after the Calculus and then ran Output to check if I ge the expected result</t>
+  </si>
+  <si>
+    <t>Entered bad input for more steps and ran flow analysis to check skips and errors</t>
+  </si>
+  <si>
+    <t>Executed Output with no previous Steps</t>
+  </si>
+  <si>
+    <t>Created a flow with each step and 2 Number Steps, executed it with some bad inputs, ran code analysis and then deleted the flow</t>
+  </si>
+  <si>
+    <t>1. TextFile(description1)()(0)</t>
+  </si>
+  <si>
+    <t>2. CsvFile(description2)()(0)</t>
+  </si>
+  <si>
+    <t>3. Display()()(1)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Skipped both previous file Steps and then executed Display to see what would be available to be displayed </t>
   </si>
 </sst>
 </file>
@@ -533,16 +614,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9860AD5-340A-E648-BB08-C399B6BE8383}">
-  <dimension ref="A1:F24"/>
+  <dimension ref="A1:F49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="E33" activeCellId="1" sqref="B38 E33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="31" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="31.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="33.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="35.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="40.6640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="33" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="30.5" bestFit="1" customWidth="1"/>
@@ -555,197 +636,174 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
         <v>1</v>
       </c>
-      <c r="B4" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A5">
-        <v>1</v>
-      </c>
-      <c r="B5" t="s">
-        <v>2</v>
-      </c>
-      <c r="C5" t="s">
-        <v>3</v>
-      </c>
-      <c r="D5" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A6">
-        <v>2</v>
-      </c>
       <c r="B6" t="s">
-        <v>5</v>
-      </c>
-      <c r="C6" t="s">
-        <v>6</v>
-      </c>
-      <c r="D6" t="s">
-        <v>7</v>
+        <v>19</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7">
+        <v>1</v>
+      </c>
+      <c r="B7" t="s">
+        <v>2</v>
+      </c>
+      <c r="C7" t="s">
         <v>3</v>
       </c>
-      <c r="B7" t="s">
-        <v>8</v>
-      </c>
-      <c r="C7" t="s">
-        <v>9</v>
-      </c>
       <c r="D7" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B8" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="C8" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="D8" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B9" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="C9" t="s">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="D9" t="s">
-        <v>14</v>
-      </c>
-      <c r="E9" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B10" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="C10" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="D10" t="s">
-        <v>16</v>
-      </c>
-      <c r="E10" t="s">
-        <v>17</v>
-      </c>
-      <c r="F10" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B11" t="s">
-        <v>19</v>
+        <v>2</v>
       </c>
       <c r="C11" t="s">
-        <v>22</v>
+        <v>3</v>
       </c>
       <c r="D11" t="s">
-        <v>21</v>
+        <v>4</v>
+      </c>
+      <c r="E11" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B12" t="s">
-        <v>23</v>
+        <v>5</v>
+      </c>
+      <c r="C12" t="s">
+        <v>6</v>
+      </c>
+      <c r="D12" t="s">
+        <v>15</v>
+      </c>
+      <c r="E12" t="s">
+        <v>16</v>
+      </c>
+      <c r="F12" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B13" t="s">
-        <v>2</v>
+        <v>18</v>
       </c>
       <c r="C13" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="D13" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B14" t="s">
-        <v>47</v>
+        <v>72</v>
       </c>
       <c r="C14" t="s">
-        <v>48</v>
+        <v>73</v>
       </c>
       <c r="D14" t="s">
-        <v>26</v>
+        <v>74</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B15" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="C15" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="D15" t="s">
-        <v>27</v>
-      </c>
-      <c r="E15" t="s">
-        <v>28</v>
-      </c>
-      <c r="F15" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B16" t="s">
-        <v>31</v>
+        <v>45</v>
       </c>
       <c r="C16" t="s">
-        <v>32</v>
+        <v>46</v>
       </c>
       <c r="D16" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B17" t="s">
         <v>8</v>
@@ -754,93 +812,310 @@
         <v>9</v>
       </c>
       <c r="D17" t="s">
-        <v>34</v>
+        <v>25</v>
+      </c>
+      <c r="E17" t="s">
+        <v>26</v>
+      </c>
+      <c r="F17" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B18" t="s">
-        <v>35</v>
+        <v>29</v>
+      </c>
+      <c r="C18" t="s">
+        <v>30</v>
+      </c>
+      <c r="D18" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B19" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="C19" t="s">
-        <v>37</v>
+        <v>9</v>
       </c>
       <c r="D19" t="s">
-        <v>36</v>
-      </c>
-      <c r="E19" t="s">
-        <v>15</v>
+        <v>32</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B20" t="s">
-        <v>38</v>
-      </c>
-      <c r="C20" t="s">
-        <v>39</v>
-      </c>
-      <c r="D20" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B21" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C21" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="D21" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="E21" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B22" t="s">
-        <v>8</v>
+        <v>36</v>
       </c>
       <c r="C22" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="D22" t="s">
-        <v>43</v>
-      </c>
-      <c r="E22" t="s">
-        <v>45</v>
-      </c>
-      <c r="F22" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23">
-        <v>19</v>
+        <v>17</v>
+      </c>
+      <c r="B23" t="s">
+        <v>5</v>
+      </c>
+      <c r="C23" t="s">
+        <v>38</v>
+      </c>
+      <c r="D23" t="s">
+        <v>40</v>
+      </c>
+      <c r="E23" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24">
+        <v>18</v>
+      </c>
+      <c r="B24" t="s">
+        <v>8</v>
+      </c>
+      <c r="C24" t="s">
+        <v>42</v>
+      </c>
+      <c r="D24" t="s">
+        <v>41</v>
+      </c>
+      <c r="E24" t="s">
+        <v>43</v>
+      </c>
+      <c r="F24" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A25">
+        <v>19</v>
+      </c>
+      <c r="B25" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A26">
         <v>20</v>
+      </c>
+      <c r="B26" t="s">
+        <v>48</v>
+      </c>
+      <c r="C26" t="s">
+        <v>49</v>
+      </c>
+      <c r="D26" t="s">
+        <v>20</v>
+      </c>
+      <c r="E26" t="s">
+        <v>50</v>
+      </c>
+      <c r="F26" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A30">
+        <v>1</v>
+      </c>
+      <c r="B30" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A31">
+        <v>2</v>
+      </c>
+      <c r="B31" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A32">
+        <v>3</v>
+      </c>
+      <c r="B32" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A33">
+        <v>4</v>
+      </c>
+      <c r="B33" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A34">
+        <v>5</v>
+      </c>
+      <c r="B34" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A35">
+        <v>6</v>
+      </c>
+      <c r="B35" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A36">
+        <v>7</v>
+      </c>
+      <c r="B36" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A37">
+        <v>8</v>
+      </c>
+      <c r="B37" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A38">
+        <v>9</v>
+      </c>
+      <c r="B38" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A39">
+        <v>10</v>
+      </c>
+      <c r="B39" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A40">
+        <v>11</v>
+      </c>
+      <c r="B40" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A41">
+        <v>12</v>
+      </c>
+      <c r="B41" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A42">
+        <v>13</v>
+      </c>
+      <c r="B42" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A43">
+        <v>14</v>
+      </c>
+      <c r="B43" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A44">
+        <v>15</v>
+      </c>
+      <c r="B44" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A45">
+        <v>16</v>
+      </c>
+      <c r="B45" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A46">
+        <v>17</v>
+      </c>
+      <c r="B46" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A47">
+        <v>18</v>
+      </c>
+      <c r="B47" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A48">
+        <v>19</v>
+      </c>
+      <c r="B48" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A49">
+        <v>20</v>
+      </c>
+      <c r="B49" t="s">
+        <v>71</v>
       </c>
     </row>
   </sheetData>

</xml_diff>